<commit_message>
Updated layout of DUNEXMainExp_MetaData.xlsx to better match the order of the missionReport and the flow of thoughts.
</commit_message>
<xml_diff>
--- a/DUNEXMainExp_MetaData.xlsx
+++ b/DUNEXMainExp_MetaData.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11012"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10912"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Volumes/DUNEXdata/DUNEXMainExp_Oct2021/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/edwinrainville/Documents/UW/DUNEX/DUNEXMainExp/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4A5A4E8D-71D5-9D40-AB23-27B7AC281D16}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{73C7D9CA-25C7-9448-ABF3-D781774BE318}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="38400" windowHeight="21600" activeTab="1" xr2:uid="{EB3AE160-BCBD-8143-A8BA-8E84C45D4E8F}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="17500" xr2:uid="{EB3AE160-BCBD-8143-A8BA-8E84C45D4E8F}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="97" uniqueCount="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="97" uniqueCount="37">
   <si>
     <t>Mission Number</t>
   </si>
@@ -98,9 +98,6 @@
   </si>
   <si>
     <t>Surf Board</t>
-  </si>
-  <si>
-    <t>EJ Rainville, 2:31 PT</t>
   </si>
   <si>
     <t>11,21,25,31,32,41</t>
@@ -254,7 +251,7 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="10">
+  <dxfs count="8">
     <dxf>
       <fill>
         <patternFill>
@@ -290,20 +287,6 @@
       <fill>
         <patternFill>
           <bgColor rgb="FF00B050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
         </patternFill>
       </fill>
     </dxf>
@@ -640,8 +623,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0EC5743F-24DA-014A-A99E-B60CA7AB8951}">
   <dimension ref="A1:X46"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+    <sheetView tabSelected="1" topLeftCell="G1" workbookViewId="0">
+      <selection activeCell="M5" sqref="M5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -679,10 +662,10 @@
         <v>22</v>
       </c>
       <c r="E1" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="F1" s="3" t="s">
         <v>4</v>
-      </c>
-      <c r="F1" s="3" t="s">
-        <v>5</v>
       </c>
       <c r="G1" s="3" t="s">
         <v>7</v>
@@ -703,7 +686,7 @@
         <v>3</v>
       </c>
       <c r="M1" s="3" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="N1" s="3" t="s">
         <v>1</v>
@@ -730,13 +713,13 @@
         <v>16</v>
       </c>
       <c r="V1" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="W1" s="3" t="s">
         <v>30</v>
       </c>
-      <c r="W1" s="3" t="s">
+      <c r="X1" s="3" t="s">
         <v>31</v>
-      </c>
-      <c r="X1" s="3" t="s">
-        <v>32</v>
       </c>
     </row>
     <row r="2" spans="1:24" ht="34" x14ac:dyDescent="0.2">
@@ -753,10 +736,10 @@
         <v>90</v>
       </c>
       <c r="E2" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="F2" s="2" t="s">
         <v>17</v>
-      </c>
-      <c r="F2" s="2" t="s">
-        <v>23</v>
       </c>
       <c r="G2" s="2" t="s">
         <v>19</v>
@@ -771,22 +754,22 @@
         <v>18</v>
       </c>
       <c r="K2" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="L2" s="5" t="s">
         <v>24</v>
-      </c>
-      <c r="L2" s="5" t="s">
-        <v>25</v>
       </c>
       <c r="M2" s="5">
         <v>6</v>
       </c>
       <c r="N2" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="O2" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="O2" s="2" t="s">
+      <c r="P2" s="5" t="s">
         <v>28</v>
-      </c>
-      <c r="P2" s="5" t="s">
-        <v>29</v>
       </c>
       <c r="Q2" s="2"/>
       <c r="R2" s="5"/>
@@ -1942,19 +1925,14 @@
       <c r="X46" s="1"/>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="A2:A46 K2:O46">
-    <cfRule type="containsBlanks" dxfId="8" priority="8">
+  <conditionalFormatting sqref="A2:A46 E2:O46">
+    <cfRule type="containsBlanks" dxfId="7" priority="8">
       <formula>LEN(TRIM(A2))=0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B2:D46">
-    <cfRule type="containsBlanks" dxfId="7" priority="7">
+  <conditionalFormatting sqref="B2:E46">
+    <cfRule type="containsBlanks" dxfId="6" priority="7">
       <formula>LEN(TRIM(B2))=0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E2:J46">
-    <cfRule type="containsBlanks" dxfId="6" priority="6">
-      <formula>LEN(TRIM(E2))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="P2:R46">
@@ -1983,7 +1961,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5BBC2C10-2C0F-BE4E-B55B-FB92E38AA170}">
   <dimension ref="A1:B66"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A33" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D68" sqref="C68:D68"/>
     </sheetView>
   </sheetViews>
@@ -1995,7 +1973,7 @@
   <sheetData>
     <row r="1" spans="1:2" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A1" s="8" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B1" s="8"/>
     </row>
@@ -2004,7 +1982,7 @@
         <v>2</v>
       </c>
       <c r="B2" s="7" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.2">
@@ -2012,7 +1990,7 @@
         <v>3</v>
       </c>
       <c r="B3" s="6" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.2">
@@ -2020,7 +1998,7 @@
         <v>4</v>
       </c>
       <c r="B4" s="6" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.2">
@@ -2028,7 +2006,7 @@
         <v>5</v>
       </c>
       <c r="B5" s="6" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.2">
@@ -2036,7 +2014,7 @@
         <v>6</v>
       </c>
       <c r="B6" s="6" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.2">
@@ -2044,7 +2022,7 @@
         <v>7</v>
       </c>
       <c r="B7" s="6" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.2">
@@ -2052,7 +2030,7 @@
         <v>8</v>
       </c>
       <c r="B8" s="6" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.2">
@@ -2060,7 +2038,7 @@
         <v>9</v>
       </c>
       <c r="B9" s="6" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.2">
@@ -2074,7 +2052,7 @@
         <v>11</v>
       </c>
       <c r="B11" s="6" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.2">
@@ -2082,7 +2060,7 @@
         <v>12</v>
       </c>
       <c r="B12" s="6" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.2">
@@ -2090,7 +2068,7 @@
         <v>13</v>
       </c>
       <c r="B13" s="6" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.2">
@@ -2104,7 +2082,7 @@
         <v>15</v>
       </c>
       <c r="B15" s="6" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.2">
@@ -2112,7 +2090,7 @@
         <v>16</v>
       </c>
       <c r="B16" s="6" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.2">
@@ -2120,7 +2098,7 @@
         <v>17</v>
       </c>
       <c r="B17" s="6" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.2">
@@ -2128,7 +2106,7 @@
         <v>18</v>
       </c>
       <c r="B18" s="6" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.2">
@@ -2136,7 +2114,7 @@
         <v>19</v>
       </c>
       <c r="B19" s="6" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.2">
@@ -2144,7 +2122,7 @@
         <v>20</v>
       </c>
       <c r="B20" s="6" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.2">
@@ -2152,7 +2130,7 @@
         <v>21</v>
       </c>
       <c r="B21" s="6" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.2">
@@ -2160,7 +2138,7 @@
         <v>22</v>
       </c>
       <c r="B22" s="6" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.2">
@@ -2168,7 +2146,7 @@
         <v>23</v>
       </c>
       <c r="B23" s="6" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.2">
@@ -2176,7 +2154,7 @@
         <v>24</v>
       </c>
       <c r="B24" s="6" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.2">
@@ -2184,7 +2162,7 @@
         <v>25</v>
       </c>
       <c r="B25" s="6" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.2">
@@ -2192,7 +2170,7 @@
         <v>26</v>
       </c>
       <c r="B26" s="6" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.2">
@@ -2200,7 +2178,7 @@
         <v>27</v>
       </c>
       <c r="B27" s="6" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.2">
@@ -2208,7 +2186,7 @@
         <v>28</v>
       </c>
       <c r="B28" s="6" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.2">
@@ -2216,7 +2194,7 @@
         <v>29</v>
       </c>
       <c r="B29" s="6" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.2">
@@ -2224,7 +2202,7 @@
         <v>30</v>
       </c>
       <c r="B30" s="6" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="31" spans="1:2" x14ac:dyDescent="0.2">
@@ -2232,7 +2210,7 @@
         <v>31</v>
       </c>
       <c r="B31" s="6" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="32" spans="1:2" x14ac:dyDescent="0.2">
@@ -2240,7 +2218,7 @@
         <v>32</v>
       </c>
       <c r="B32" s="6" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="33" spans="1:2" x14ac:dyDescent="0.2">
@@ -2248,7 +2226,7 @@
         <v>33</v>
       </c>
       <c r="B33" s="6" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="34" spans="1:2" x14ac:dyDescent="0.2">
@@ -2256,7 +2234,7 @@
         <v>34</v>
       </c>
       <c r="B34" s="6" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="35" spans="1:2" x14ac:dyDescent="0.2">
@@ -2264,7 +2242,7 @@
         <v>35</v>
       </c>
       <c r="B35" s="6" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="36" spans="1:2" x14ac:dyDescent="0.2">
@@ -2272,7 +2250,7 @@
         <v>36</v>
       </c>
       <c r="B36" s="6" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="37" spans="1:2" x14ac:dyDescent="0.2">
@@ -2280,7 +2258,7 @@
         <v>37</v>
       </c>
       <c r="B37" s="6" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="38" spans="1:2" x14ac:dyDescent="0.2">
@@ -2288,7 +2266,7 @@
         <v>38</v>
       </c>
       <c r="B38" s="6" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="39" spans="1:2" x14ac:dyDescent="0.2">
@@ -2296,7 +2274,7 @@
         <v>39</v>
       </c>
       <c r="B39" s="6" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="40" spans="1:2" x14ac:dyDescent="0.2">
@@ -2304,7 +2282,7 @@
         <v>40</v>
       </c>
       <c r="B40" s="6" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="41" spans="1:2" x14ac:dyDescent="0.2">
@@ -2312,7 +2290,7 @@
         <v>41</v>
       </c>
       <c r="B41" s="6" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="42" spans="1:2" x14ac:dyDescent="0.2">
@@ -2320,7 +2298,7 @@
         <v>42</v>
       </c>
       <c r="B42" s="6" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="43" spans="1:2" x14ac:dyDescent="0.2">
@@ -2328,7 +2306,7 @@
         <v>43</v>
       </c>
       <c r="B43" s="6" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="44" spans="1:2" x14ac:dyDescent="0.2">
@@ -2336,7 +2314,7 @@
         <v>44</v>
       </c>
       <c r="B44" s="6" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="45" spans="1:2" x14ac:dyDescent="0.2">
@@ -2344,7 +2322,7 @@
         <v>45</v>
       </c>
       <c r="B45" s="6" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="46" spans="1:2" x14ac:dyDescent="0.2">
@@ -2358,7 +2336,7 @@
         <v>47</v>
       </c>
       <c r="B47" s="6" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="48" spans="1:2" x14ac:dyDescent="0.2">
@@ -2366,7 +2344,7 @@
         <v>48</v>
       </c>
       <c r="B48" s="6" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="49" spans="1:2" x14ac:dyDescent="0.2">
@@ -2374,7 +2352,7 @@
         <v>49</v>
       </c>
       <c r="B49" s="6" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="50" spans="1:2" x14ac:dyDescent="0.2">
@@ -2382,7 +2360,7 @@
         <v>50</v>
       </c>
       <c r="B50" s="6" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="51" spans="1:2" x14ac:dyDescent="0.2">
@@ -2390,7 +2368,7 @@
         <v>51</v>
       </c>
       <c r="B51" s="6" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="52" spans="1:2" x14ac:dyDescent="0.2">
@@ -2398,7 +2376,7 @@
         <v>52</v>
       </c>
       <c r="B52" s="6" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="53" spans="1:2" x14ac:dyDescent="0.2">
@@ -2406,7 +2384,7 @@
         <v>53</v>
       </c>
       <c r="B53" s="6" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="54" spans="1:2" x14ac:dyDescent="0.2">
@@ -2414,7 +2392,7 @@
         <v>54</v>
       </c>
       <c r="B54" s="6" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="55" spans="1:2" x14ac:dyDescent="0.2">
@@ -2422,7 +2400,7 @@
         <v>55</v>
       </c>
       <c r="B55" s="6" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="56" spans="1:2" x14ac:dyDescent="0.2">
@@ -2430,7 +2408,7 @@
         <v>56</v>
       </c>
       <c r="B56" s="6" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="57" spans="1:2" x14ac:dyDescent="0.2">
@@ -2438,7 +2416,7 @@
         <v>57</v>
       </c>
       <c r="B57" s="6" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="58" spans="1:2" x14ac:dyDescent="0.2">
@@ -2446,7 +2424,7 @@
         <v>58</v>
       </c>
       <c r="B58" s="6" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="59" spans="1:2" x14ac:dyDescent="0.2">
@@ -2454,7 +2432,7 @@
         <v>59</v>
       </c>
       <c r="B59" s="6" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="60" spans="1:2" x14ac:dyDescent="0.2">
@@ -2462,7 +2440,7 @@
         <v>60</v>
       </c>
       <c r="B60" s="6" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="61" spans="1:2" x14ac:dyDescent="0.2">
@@ -2470,7 +2448,7 @@
         <v>61</v>
       </c>
       <c r="B61" s="6" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="62" spans="1:2" x14ac:dyDescent="0.2">
@@ -2478,7 +2456,7 @@
         <v>62</v>
       </c>
       <c r="B62" s="6" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="63" spans="1:2" x14ac:dyDescent="0.2">
@@ -2486,7 +2464,7 @@
         <v>63</v>
       </c>
       <c r="B63" s="6" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="64" spans="1:2" x14ac:dyDescent="0.2">
@@ -2500,7 +2478,7 @@
         <v>65</v>
       </c>
       <c r="B65" s="6" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="66" spans="1:2" x14ac:dyDescent="0.2">
@@ -2508,7 +2486,7 @@
         <v>66</v>
       </c>
       <c r="B66" s="6" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added some more info to the metadata spreadsheet to test the missionReport script
</commit_message>
<xml_diff>
--- a/DUNEXMainExp_MetaData.xlsx
+++ b/DUNEXMainExp_MetaData.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/edwinrainville/Documents/UW/DUNEX/DUNEXMainExp/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{73C7D9CA-25C7-9448-ABF3-D781774BE318}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{25E4ED18-16DF-EB4C-946B-D40CF8AE1C57}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="17500" xr2:uid="{EB3AE160-BCBD-8143-A8BA-8E84C45D4E8F}"/>
   </bookViews>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="97" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="99" uniqueCount="38">
   <si>
     <t>Mission Number</t>
   </si>
@@ -46,27 +46,12 @@
     <t>Deployment Method</t>
   </si>
   <si>
-    <t>microSWIFT turn on and check</t>
-  </si>
-  <si>
     <t>Lead Deployer</t>
   </si>
   <si>
-    <t>Assistant Deployer</t>
-  </si>
-  <si>
-    <t>Lead Note Taker</t>
-  </si>
-  <si>
-    <t>Assitant Note Taker</t>
-  </si>
-  <si>
     <t>Deployment Notes</t>
   </si>
   <si>
-    <t>Data Offloaded and Archived</t>
-  </si>
-  <si>
     <t>Data Offload Notes</t>
   </si>
   <si>
@@ -82,9 +67,6 @@
     <t>Lab Bench</t>
   </si>
   <si>
-    <t>N/A</t>
-  </si>
-  <si>
     <t>EJ Rainville</t>
   </si>
   <si>
@@ -137,6 +119,27 @@
   </si>
   <si>
     <t>NO BOARD</t>
+  </si>
+  <si>
+    <t>Aide</t>
+  </si>
+  <si>
+    <t>Notetaker</t>
+  </si>
+  <si>
+    <t>microSWIFTs checked by</t>
+  </si>
+  <si>
+    <t>Data Offloaded and Archived by</t>
+  </si>
+  <si>
+    <t>All data offloaded correctly</t>
+  </si>
+  <si>
+    <t>Lead Retriever</t>
+  </si>
+  <si>
+    <t>Emily Iseley</t>
   </si>
 </sst>
 </file>
@@ -623,8 +626,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0EC5743F-24DA-014A-A99E-B60CA7AB8951}">
   <dimension ref="A1:X46"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="G1" workbookViewId="0">
-      <selection activeCell="M5" sqref="M5"/>
+    <sheetView tabSelected="1" topLeftCell="F1" workbookViewId="0">
+      <selection activeCell="K5" sqref="K5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -639,7 +642,8 @@
     <col min="13" max="13" width="26.33203125" bestFit="1" customWidth="1"/>
     <col min="14" max="15" width="18.6640625" bestFit="1" customWidth="1"/>
     <col min="16" max="16" width="31.33203125" customWidth="1"/>
-    <col min="17" max="18" width="25" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="27.5" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="25" bestFit="1" customWidth="1"/>
     <col min="19" max="19" width="30.5" bestFit="1" customWidth="1"/>
     <col min="20" max="20" width="30.83203125" bestFit="1" customWidth="1"/>
     <col min="21" max="21" width="13.6640625" bestFit="1" customWidth="1"/>
@@ -653,13 +657,13 @@
         <v>0</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>20</v>
+        <v>14</v>
       </c>
       <c r="C1" s="3" t="s">
-        <v>21</v>
+        <v>15</v>
       </c>
       <c r="D1" s="3" t="s">
-        <v>22</v>
+        <v>16</v>
       </c>
       <c r="E1" s="3" t="s">
         <v>5</v>
@@ -668,25 +672,25 @@
         <v>4</v>
       </c>
       <c r="G1" s="3" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="H1" s="3" t="s">
-        <v>8</v>
+        <v>36</v>
       </c>
       <c r="I1" s="3" t="s">
-        <v>9</v>
+        <v>31</v>
       </c>
       <c r="J1" s="3" t="s">
-        <v>10</v>
+        <v>32</v>
       </c>
       <c r="K1" s="3" t="s">
-        <v>6</v>
+        <v>33</v>
       </c>
       <c r="L1" s="3" t="s">
         <v>3</v>
       </c>
       <c r="M1" s="3" t="s">
-        <v>25</v>
+        <v>19</v>
       </c>
       <c r="N1" s="3" t="s">
         <v>1</v>
@@ -695,31 +699,31 @@
         <v>2</v>
       </c>
       <c r="P1" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="Q1" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="R1" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="S1" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="T1" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="U1" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="Q1" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="R1" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="S1" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="T1" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="U1" s="3" t="s">
-        <v>16</v>
-      </c>
       <c r="V1" s="3" t="s">
-        <v>29</v>
+        <v>23</v>
       </c>
       <c r="W1" s="3" t="s">
-        <v>30</v>
+        <v>24</v>
       </c>
       <c r="X1" s="3" t="s">
-        <v>31</v>
+        <v>25</v>
       </c>
     </row>
     <row r="2" spans="1:24" ht="34" x14ac:dyDescent="0.2">
@@ -736,43 +740,47 @@
         <v>90</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>23</v>
+        <v>17</v>
       </c>
       <c r="F2" s="2" t="s">
-        <v>17</v>
+        <v>12</v>
       </c>
       <c r="G2" s="2" t="s">
-        <v>19</v>
+        <v>13</v>
       </c>
       <c r="H2" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="I2" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="J2" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="K2" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="L2" s="5" t="s">
         <v>18</v>
-      </c>
-      <c r="I2" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="J2" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="K2" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="L2" s="5" t="s">
-        <v>24</v>
       </c>
       <c r="M2" s="5">
         <v>6</v>
       </c>
       <c r="N2" s="2" t="s">
-        <v>26</v>
+        <v>20</v>
       </c>
       <c r="O2" s="2" t="s">
-        <v>27</v>
+        <v>21</v>
       </c>
       <c r="P2" s="5" t="s">
-        <v>28</v>
-      </c>
-      <c r="Q2" s="2"/>
-      <c r="R2" s="5"/>
+        <v>22</v>
+      </c>
+      <c r="Q2" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="R2" s="5" t="s">
+        <v>35</v>
+      </c>
       <c r="S2" s="2"/>
       <c r="T2" s="2"/>
       <c r="U2" s="2"/>
@@ -1973,7 +1981,7 @@
   <sheetData>
     <row r="1" spans="1:2" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A1" s="8" t="s">
-        <v>32</v>
+        <v>26</v>
       </c>
       <c r="B1" s="8"/>
     </row>
@@ -1982,7 +1990,7 @@
         <v>2</v>
       </c>
       <c r="B2" s="7" t="s">
-        <v>33</v>
+        <v>27</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.2">
@@ -1990,7 +1998,7 @@
         <v>3</v>
       </c>
       <c r="B3" s="6" t="s">
-        <v>33</v>
+        <v>27</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.2">
@@ -1998,7 +2006,7 @@
         <v>4</v>
       </c>
       <c r="B4" s="6" t="s">
-        <v>33</v>
+        <v>27</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.2">
@@ -2006,7 +2014,7 @@
         <v>5</v>
       </c>
       <c r="B5" s="6" t="s">
-        <v>33</v>
+        <v>27</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.2">
@@ -2014,7 +2022,7 @@
         <v>6</v>
       </c>
       <c r="B6" s="6" t="s">
-        <v>33</v>
+        <v>27</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.2">
@@ -2022,7 +2030,7 @@
         <v>7</v>
       </c>
       <c r="B7" s="6" t="s">
-        <v>33</v>
+        <v>27</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.2">
@@ -2030,7 +2038,7 @@
         <v>8</v>
       </c>
       <c r="B8" s="6" t="s">
-        <v>33</v>
+        <v>27</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.2">
@@ -2038,7 +2046,7 @@
         <v>9</v>
       </c>
       <c r="B9" s="6" t="s">
-        <v>33</v>
+        <v>27</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.2">
@@ -2052,7 +2060,7 @@
         <v>11</v>
       </c>
       <c r="B11" s="6" t="s">
-        <v>33</v>
+        <v>27</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.2">
@@ -2060,7 +2068,7 @@
         <v>12</v>
       </c>
       <c r="B12" s="6" t="s">
-        <v>33</v>
+        <v>27</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.2">
@@ -2068,7 +2076,7 @@
         <v>13</v>
       </c>
       <c r="B13" s="6" t="s">
-        <v>33</v>
+        <v>27</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.2">
@@ -2082,7 +2090,7 @@
         <v>15</v>
       </c>
       <c r="B15" s="6" t="s">
-        <v>33</v>
+        <v>27</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.2">
@@ -2090,7 +2098,7 @@
         <v>16</v>
       </c>
       <c r="B16" s="6" t="s">
-        <v>33</v>
+        <v>27</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.2">
@@ -2098,7 +2106,7 @@
         <v>17</v>
       </c>
       <c r="B17" s="6" t="s">
-        <v>33</v>
+        <v>27</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.2">
@@ -2106,7 +2114,7 @@
         <v>18</v>
       </c>
       <c r="B18" s="6" t="s">
-        <v>33</v>
+        <v>27</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.2">
@@ -2114,7 +2122,7 @@
         <v>19</v>
       </c>
       <c r="B19" s="6" t="s">
-        <v>33</v>
+        <v>27</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.2">
@@ -2122,7 +2130,7 @@
         <v>20</v>
       </c>
       <c r="B20" s="6" t="s">
-        <v>33</v>
+        <v>27</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.2">
@@ -2130,7 +2138,7 @@
         <v>21</v>
       </c>
       <c r="B21" s="6" t="s">
-        <v>33</v>
+        <v>27</v>
       </c>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.2">
@@ -2138,7 +2146,7 @@
         <v>22</v>
       </c>
       <c r="B22" s="6" t="s">
-        <v>33</v>
+        <v>27</v>
       </c>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.2">
@@ -2146,7 +2154,7 @@
         <v>23</v>
       </c>
       <c r="B23" s="6" t="s">
-        <v>33</v>
+        <v>27</v>
       </c>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.2">
@@ -2154,7 +2162,7 @@
         <v>24</v>
       </c>
       <c r="B24" s="6" t="s">
-        <v>33</v>
+        <v>27</v>
       </c>
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.2">
@@ -2162,7 +2170,7 @@
         <v>25</v>
       </c>
       <c r="B25" s="6" t="s">
-        <v>33</v>
+        <v>27</v>
       </c>
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.2">
@@ -2170,7 +2178,7 @@
         <v>26</v>
       </c>
       <c r="B26" s="6" t="s">
-        <v>33</v>
+        <v>27</v>
       </c>
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.2">
@@ -2178,7 +2186,7 @@
         <v>27</v>
       </c>
       <c r="B27" s="6" t="s">
-        <v>33</v>
+        <v>27</v>
       </c>
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.2">
@@ -2186,7 +2194,7 @@
         <v>28</v>
       </c>
       <c r="B28" s="6" t="s">
-        <v>33</v>
+        <v>27</v>
       </c>
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.2">
@@ -2194,7 +2202,7 @@
         <v>29</v>
       </c>
       <c r="B29" s="6" t="s">
-        <v>33</v>
+        <v>27</v>
       </c>
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.2">
@@ -2202,7 +2210,7 @@
         <v>30</v>
       </c>
       <c r="B30" s="6" t="s">
-        <v>34</v>
+        <v>28</v>
       </c>
     </row>
     <row r="31" spans="1:2" x14ac:dyDescent="0.2">
@@ -2210,7 +2218,7 @@
         <v>31</v>
       </c>
       <c r="B31" s="6" t="s">
-        <v>33</v>
+        <v>27</v>
       </c>
     </row>
     <row r="32" spans="1:2" x14ac:dyDescent="0.2">
@@ -2218,7 +2226,7 @@
         <v>32</v>
       </c>
       <c r="B32" s="6" t="s">
-        <v>33</v>
+        <v>27</v>
       </c>
     </row>
     <row r="33" spans="1:2" x14ac:dyDescent="0.2">
@@ -2226,7 +2234,7 @@
         <v>33</v>
       </c>
       <c r="B33" s="6" t="s">
-        <v>33</v>
+        <v>27</v>
       </c>
     </row>
     <row r="34" spans="1:2" x14ac:dyDescent="0.2">
@@ -2234,7 +2242,7 @@
         <v>34</v>
       </c>
       <c r="B34" s="6" t="s">
-        <v>33</v>
+        <v>27</v>
       </c>
     </row>
     <row r="35" spans="1:2" x14ac:dyDescent="0.2">
@@ -2242,7 +2250,7 @@
         <v>35</v>
       </c>
       <c r="B35" s="6" t="s">
-        <v>33</v>
+        <v>27</v>
       </c>
     </row>
     <row r="36" spans="1:2" x14ac:dyDescent="0.2">
@@ -2250,7 +2258,7 @@
         <v>36</v>
       </c>
       <c r="B36" s="6" t="s">
-        <v>33</v>
+        <v>27</v>
       </c>
     </row>
     <row r="37" spans="1:2" x14ac:dyDescent="0.2">
@@ -2258,7 +2266,7 @@
         <v>37</v>
       </c>
       <c r="B37" s="6" t="s">
-        <v>33</v>
+        <v>27</v>
       </c>
     </row>
     <row r="38" spans="1:2" x14ac:dyDescent="0.2">
@@ -2266,7 +2274,7 @@
         <v>38</v>
       </c>
       <c r="B38" s="6" t="s">
-        <v>33</v>
+        <v>27</v>
       </c>
     </row>
     <row r="39" spans="1:2" x14ac:dyDescent="0.2">
@@ -2274,7 +2282,7 @@
         <v>39</v>
       </c>
       <c r="B39" s="6" t="s">
-        <v>33</v>
+        <v>27</v>
       </c>
     </row>
     <row r="40" spans="1:2" x14ac:dyDescent="0.2">
@@ -2282,7 +2290,7 @@
         <v>40</v>
       </c>
       <c r="B40" s="6" t="s">
-        <v>33</v>
+        <v>27</v>
       </c>
     </row>
     <row r="41" spans="1:2" x14ac:dyDescent="0.2">
@@ -2290,7 +2298,7 @@
         <v>41</v>
       </c>
       <c r="B41" s="6" t="s">
-        <v>33</v>
+        <v>27</v>
       </c>
     </row>
     <row r="42" spans="1:2" x14ac:dyDescent="0.2">
@@ -2298,7 +2306,7 @@
         <v>42</v>
       </c>
       <c r="B42" s="6" t="s">
-        <v>33</v>
+        <v>27</v>
       </c>
     </row>
     <row r="43" spans="1:2" x14ac:dyDescent="0.2">
@@ -2306,7 +2314,7 @@
         <v>43</v>
       </c>
       <c r="B43" s="6" t="s">
-        <v>33</v>
+        <v>27</v>
       </c>
     </row>
     <row r="44" spans="1:2" x14ac:dyDescent="0.2">
@@ -2314,7 +2322,7 @@
         <v>44</v>
       </c>
       <c r="B44" s="6" t="s">
-        <v>33</v>
+        <v>27</v>
       </c>
     </row>
     <row r="45" spans="1:2" x14ac:dyDescent="0.2">
@@ -2322,7 +2330,7 @@
         <v>45</v>
       </c>
       <c r="B45" s="6" t="s">
-        <v>33</v>
+        <v>27</v>
       </c>
     </row>
     <row r="46" spans="1:2" x14ac:dyDescent="0.2">
@@ -2336,7 +2344,7 @@
         <v>47</v>
       </c>
       <c r="B47" s="6" t="s">
-        <v>33</v>
+        <v>27</v>
       </c>
     </row>
     <row r="48" spans="1:2" x14ac:dyDescent="0.2">
@@ -2344,7 +2352,7 @@
         <v>48</v>
       </c>
       <c r="B48" s="6" t="s">
-        <v>33</v>
+        <v>27</v>
       </c>
     </row>
     <row r="49" spans="1:2" x14ac:dyDescent="0.2">
@@ -2352,7 +2360,7 @@
         <v>49</v>
       </c>
       <c r="B49" s="6" t="s">
-        <v>33</v>
+        <v>27</v>
       </c>
     </row>
     <row r="50" spans="1:2" x14ac:dyDescent="0.2">
@@ -2360,7 +2368,7 @@
         <v>50</v>
       </c>
       <c r="B50" s="6" t="s">
-        <v>33</v>
+        <v>27</v>
       </c>
     </row>
     <row r="51" spans="1:2" x14ac:dyDescent="0.2">
@@ -2368,7 +2376,7 @@
         <v>51</v>
       </c>
       <c r="B51" s="6" t="s">
-        <v>35</v>
+        <v>29</v>
       </c>
     </row>
     <row r="52" spans="1:2" x14ac:dyDescent="0.2">
@@ -2376,7 +2384,7 @@
         <v>52</v>
       </c>
       <c r="B52" s="6" t="s">
-        <v>35</v>
+        <v>29</v>
       </c>
     </row>
     <row r="53" spans="1:2" x14ac:dyDescent="0.2">
@@ -2384,7 +2392,7 @@
         <v>53</v>
       </c>
       <c r="B53" s="6" t="s">
-        <v>35</v>
+        <v>29</v>
       </c>
     </row>
     <row r="54" spans="1:2" x14ac:dyDescent="0.2">
@@ -2392,7 +2400,7 @@
         <v>54</v>
       </c>
       <c r="B54" s="6" t="s">
-        <v>33</v>
+        <v>27</v>
       </c>
     </row>
     <row r="55" spans="1:2" x14ac:dyDescent="0.2">
@@ -2400,7 +2408,7 @@
         <v>55</v>
       </c>
       <c r="B55" s="6" t="s">
-        <v>35</v>
+        <v>29</v>
       </c>
     </row>
     <row r="56" spans="1:2" x14ac:dyDescent="0.2">
@@ -2408,7 +2416,7 @@
         <v>56</v>
       </c>
       <c r="B56" s="6" t="s">
-        <v>33</v>
+        <v>27</v>
       </c>
     </row>
     <row r="57" spans="1:2" x14ac:dyDescent="0.2">
@@ -2416,7 +2424,7 @@
         <v>57</v>
       </c>
       <c r="B57" s="6" t="s">
-        <v>33</v>
+        <v>27</v>
       </c>
     </row>
     <row r="58" spans="1:2" x14ac:dyDescent="0.2">
@@ -2424,7 +2432,7 @@
         <v>58</v>
       </c>
       <c r="B58" s="6" t="s">
-        <v>33</v>
+        <v>27</v>
       </c>
     </row>
     <row r="59" spans="1:2" x14ac:dyDescent="0.2">
@@ -2432,7 +2440,7 @@
         <v>59</v>
       </c>
       <c r="B59" s="6" t="s">
-        <v>33</v>
+        <v>27</v>
       </c>
     </row>
     <row r="60" spans="1:2" x14ac:dyDescent="0.2">
@@ -2440,7 +2448,7 @@
         <v>60</v>
       </c>
       <c r="B60" s="6" t="s">
-        <v>33</v>
+        <v>27</v>
       </c>
     </row>
     <row r="61" spans="1:2" x14ac:dyDescent="0.2">
@@ -2448,7 +2456,7 @@
         <v>61</v>
       </c>
       <c r="B61" s="6" t="s">
-        <v>33</v>
+        <v>27</v>
       </c>
     </row>
     <row r="62" spans="1:2" x14ac:dyDescent="0.2">
@@ -2456,7 +2464,7 @@
         <v>62</v>
       </c>
       <c r="B62" s="6" t="s">
-        <v>33</v>
+        <v>27</v>
       </c>
     </row>
     <row r="63" spans="1:2" x14ac:dyDescent="0.2">
@@ -2464,7 +2472,7 @@
         <v>63</v>
       </c>
       <c r="B63" s="6" t="s">
-        <v>36</v>
+        <v>30</v>
       </c>
     </row>
     <row r="64" spans="1:2" x14ac:dyDescent="0.2">
@@ -2478,7 +2486,7 @@
         <v>65</v>
       </c>
       <c r="B65" s="6" t="s">
-        <v>33</v>
+        <v>27</v>
       </c>
     </row>
     <row r="66" spans="1:2" x14ac:dyDescent="0.2">
@@ -2486,7 +2494,7 @@
         <v>66</v>
       </c>
       <c r="B66" s="6" t="s">
-        <v>33</v>
+        <v>27</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Updated meetadata spreadsheet and exploration notebook
</commit_message>
<xml_diff>
--- a/DUNEXMainExp_MetaData.xlsx
+++ b/DUNEXMainExp_MetaData.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/edwinrainville/Documents/UW/DUNEX/DUNEXMainExp/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{25E4ED18-16DF-EB4C-946B-D40CF8AE1C57}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AEDD8FA3-4DB7-5144-99F4-159814B7A707}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="17500" xr2:uid="{EB3AE160-BCBD-8143-A8BA-8E84C45D4E8F}"/>
   </bookViews>
@@ -627,7 +627,7 @@
   <dimension ref="A1:X46"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="F1" workbookViewId="0">
-      <selection activeCell="K5" sqref="K5"/>
+      <selection activeCell="F4" sqref="F4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>

<commit_message>
Updated metadata to explicitly state that the first row is an example
</commit_message>
<xml_diff>
--- a/DUNEXMainExp_MetaData.xlsx
+++ b/DUNEXMainExp_MetaData.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/edwinrainville/Documents/UW/DUNEX/DUNEXMainExp/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AEDD8FA3-4DB7-5144-99F4-159814B7A707}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A539EAB9-B394-5342-A0D7-D8A16DEE8676}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="17500" xr2:uid="{EB3AE160-BCBD-8143-A8BA-8E84C45D4E8F}"/>
   </bookViews>
@@ -94,9 +94,6 @@
     <t>2021-09-21T22:30:00</t>
   </si>
   <si>
-    <t>Testing Data offload workflow on Lab bench</t>
-  </si>
-  <si>
     <t>Minimum Significant Wave Height</t>
   </si>
   <si>
@@ -133,13 +130,16 @@
     <t>Data Offloaded and Archived by</t>
   </si>
   <si>
-    <t>All data offloaded correctly</t>
-  </si>
-  <si>
     <t>Lead Retriever</t>
   </si>
   <si>
     <t>Emily Iseley</t>
+  </si>
+  <si>
+    <t>This is an example deployment. Testing Data offload workflow on Lab bench</t>
+  </si>
+  <si>
+    <t>This is an example. All data offloaded correctly</t>
   </si>
 </sst>
 </file>
@@ -626,8 +626,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0EC5743F-24DA-014A-A99E-B60CA7AB8951}">
   <dimension ref="A1:X46"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="F1" workbookViewId="0">
-      <selection activeCell="F4" sqref="F4"/>
+    <sheetView tabSelected="1" topLeftCell="K1" workbookViewId="0">
+      <selection activeCell="R3" sqref="R3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -675,16 +675,16 @@
         <v>6</v>
       </c>
       <c r="H1" s="3" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="I1" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="J1" s="3" t="s">
         <v>31</v>
       </c>
-      <c r="J1" s="3" t="s">
+      <c r="K1" s="3" t="s">
         <v>32</v>
-      </c>
-      <c r="K1" s="3" t="s">
-        <v>33</v>
       </c>
       <c r="L1" s="3" t="s">
         <v>3</v>
@@ -702,7 +702,7 @@
         <v>7</v>
       </c>
       <c r="Q1" s="3" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="R1" s="3" t="s">
         <v>8</v>
@@ -717,16 +717,16 @@
         <v>11</v>
       </c>
       <c r="V1" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="W1" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="W1" s="3" t="s">
+      <c r="X1" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="X1" s="3" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="2" spans="1:24" ht="34" x14ac:dyDescent="0.2">
+    </row>
+    <row r="2" spans="1:24" ht="51" x14ac:dyDescent="0.2">
       <c r="A2" s="2">
         <v>0</v>
       </c>
@@ -749,10 +749,10 @@
         <v>13</v>
       </c>
       <c r="H2" s="2" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="I2" s="2" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="J2" s="2" t="s">
         <v>13</v>
@@ -773,13 +773,13 @@
         <v>21</v>
       </c>
       <c r="P2" s="5" t="s">
-        <v>22</v>
+        <v>36</v>
       </c>
       <c r="Q2" s="2" t="s">
         <v>13</v>
       </c>
       <c r="R2" s="5" t="s">
-        <v>35</v>
+        <v>37</v>
       </c>
       <c r="S2" s="2"/>
       <c r="T2" s="2"/>
@@ -1981,7 +1981,7 @@
   <sheetData>
     <row r="1" spans="1:2" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A1" s="8" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B1" s="8"/>
     </row>
@@ -1990,7 +1990,7 @@
         <v>2</v>
       </c>
       <c r="B2" s="7" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.2">
@@ -1998,7 +1998,7 @@
         <v>3</v>
       </c>
       <c r="B3" s="6" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.2">
@@ -2006,7 +2006,7 @@
         <v>4</v>
       </c>
       <c r="B4" s="6" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.2">
@@ -2014,7 +2014,7 @@
         <v>5</v>
       </c>
       <c r="B5" s="6" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.2">
@@ -2022,7 +2022,7 @@
         <v>6</v>
       </c>
       <c r="B6" s="6" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.2">
@@ -2030,7 +2030,7 @@
         <v>7</v>
       </c>
       <c r="B7" s="6" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.2">
@@ -2038,7 +2038,7 @@
         <v>8</v>
       </c>
       <c r="B8" s="6" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.2">
@@ -2046,7 +2046,7 @@
         <v>9</v>
       </c>
       <c r="B9" s="6" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.2">
@@ -2060,7 +2060,7 @@
         <v>11</v>
       </c>
       <c r="B11" s="6" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.2">
@@ -2068,7 +2068,7 @@
         <v>12</v>
       </c>
       <c r="B12" s="6" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.2">
@@ -2076,7 +2076,7 @@
         <v>13</v>
       </c>
       <c r="B13" s="6" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.2">
@@ -2090,7 +2090,7 @@
         <v>15</v>
       </c>
       <c r="B15" s="6" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.2">
@@ -2098,7 +2098,7 @@
         <v>16</v>
       </c>
       <c r="B16" s="6" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.2">
@@ -2106,7 +2106,7 @@
         <v>17</v>
       </c>
       <c r="B17" s="6" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.2">
@@ -2114,7 +2114,7 @@
         <v>18</v>
       </c>
       <c r="B18" s="6" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.2">
@@ -2122,7 +2122,7 @@
         <v>19</v>
       </c>
       <c r="B19" s="6" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.2">
@@ -2130,7 +2130,7 @@
         <v>20</v>
       </c>
       <c r="B20" s="6" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.2">
@@ -2138,7 +2138,7 @@
         <v>21</v>
       </c>
       <c r="B21" s="6" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.2">
@@ -2146,7 +2146,7 @@
         <v>22</v>
       </c>
       <c r="B22" s="6" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.2">
@@ -2154,7 +2154,7 @@
         <v>23</v>
       </c>
       <c r="B23" s="6" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.2">
@@ -2162,7 +2162,7 @@
         <v>24</v>
       </c>
       <c r="B24" s="6" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.2">
@@ -2170,7 +2170,7 @@
         <v>25</v>
       </c>
       <c r="B25" s="6" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.2">
@@ -2178,7 +2178,7 @@
         <v>26</v>
       </c>
       <c r="B26" s="6" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.2">
@@ -2186,7 +2186,7 @@
         <v>27</v>
       </c>
       <c r="B27" s="6" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.2">
@@ -2194,7 +2194,7 @@
         <v>28</v>
       </c>
       <c r="B28" s="6" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.2">
@@ -2202,7 +2202,7 @@
         <v>29</v>
       </c>
       <c r="B29" s="6" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.2">
@@ -2210,7 +2210,7 @@
         <v>30</v>
       </c>
       <c r="B30" s="6" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="31" spans="1:2" x14ac:dyDescent="0.2">
@@ -2218,7 +2218,7 @@
         <v>31</v>
       </c>
       <c r="B31" s="6" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="32" spans="1:2" x14ac:dyDescent="0.2">
@@ -2226,7 +2226,7 @@
         <v>32</v>
       </c>
       <c r="B32" s="6" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="33" spans="1:2" x14ac:dyDescent="0.2">
@@ -2234,7 +2234,7 @@
         <v>33</v>
       </c>
       <c r="B33" s="6" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="34" spans="1:2" x14ac:dyDescent="0.2">
@@ -2242,7 +2242,7 @@
         <v>34</v>
       </c>
       <c r="B34" s="6" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="35" spans="1:2" x14ac:dyDescent="0.2">
@@ -2250,7 +2250,7 @@
         <v>35</v>
       </c>
       <c r="B35" s="6" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="36" spans="1:2" x14ac:dyDescent="0.2">
@@ -2258,7 +2258,7 @@
         <v>36</v>
       </c>
       <c r="B36" s="6" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="37" spans="1:2" x14ac:dyDescent="0.2">
@@ -2266,7 +2266,7 @@
         <v>37</v>
       </c>
       <c r="B37" s="6" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="38" spans="1:2" x14ac:dyDescent="0.2">
@@ -2274,7 +2274,7 @@
         <v>38</v>
       </c>
       <c r="B38" s="6" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="39" spans="1:2" x14ac:dyDescent="0.2">
@@ -2282,7 +2282,7 @@
         <v>39</v>
       </c>
       <c r="B39" s="6" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="40" spans="1:2" x14ac:dyDescent="0.2">
@@ -2290,7 +2290,7 @@
         <v>40</v>
       </c>
       <c r="B40" s="6" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="41" spans="1:2" x14ac:dyDescent="0.2">
@@ -2298,7 +2298,7 @@
         <v>41</v>
       </c>
       <c r="B41" s="6" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="42" spans="1:2" x14ac:dyDescent="0.2">
@@ -2306,7 +2306,7 @@
         <v>42</v>
       </c>
       <c r="B42" s="6" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="43" spans="1:2" x14ac:dyDescent="0.2">
@@ -2314,7 +2314,7 @@
         <v>43</v>
       </c>
       <c r="B43" s="6" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="44" spans="1:2" x14ac:dyDescent="0.2">
@@ -2322,7 +2322,7 @@
         <v>44</v>
       </c>
       <c r="B44" s="6" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="45" spans="1:2" x14ac:dyDescent="0.2">
@@ -2330,7 +2330,7 @@
         <v>45</v>
       </c>
       <c r="B45" s="6" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="46" spans="1:2" x14ac:dyDescent="0.2">
@@ -2344,7 +2344,7 @@
         <v>47</v>
       </c>
       <c r="B47" s="6" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="48" spans="1:2" x14ac:dyDescent="0.2">
@@ -2352,7 +2352,7 @@
         <v>48</v>
       </c>
       <c r="B48" s="6" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="49" spans="1:2" x14ac:dyDescent="0.2">
@@ -2360,7 +2360,7 @@
         <v>49</v>
       </c>
       <c r="B49" s="6" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="50" spans="1:2" x14ac:dyDescent="0.2">
@@ -2368,7 +2368,7 @@
         <v>50</v>
       </c>
       <c r="B50" s="6" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="51" spans="1:2" x14ac:dyDescent="0.2">
@@ -2376,7 +2376,7 @@
         <v>51</v>
       </c>
       <c r="B51" s="6" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="52" spans="1:2" x14ac:dyDescent="0.2">
@@ -2384,7 +2384,7 @@
         <v>52</v>
       </c>
       <c r="B52" s="6" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="53" spans="1:2" x14ac:dyDescent="0.2">
@@ -2392,7 +2392,7 @@
         <v>53</v>
       </c>
       <c r="B53" s="6" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="54" spans="1:2" x14ac:dyDescent="0.2">
@@ -2400,7 +2400,7 @@
         <v>54</v>
       </c>
       <c r="B54" s="6" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="55" spans="1:2" x14ac:dyDescent="0.2">
@@ -2408,7 +2408,7 @@
         <v>55</v>
       </c>
       <c r="B55" s="6" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="56" spans="1:2" x14ac:dyDescent="0.2">
@@ -2416,7 +2416,7 @@
         <v>56</v>
       </c>
       <c r="B56" s="6" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="57" spans="1:2" x14ac:dyDescent="0.2">
@@ -2424,7 +2424,7 @@
         <v>57</v>
       </c>
       <c r="B57" s="6" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="58" spans="1:2" x14ac:dyDescent="0.2">
@@ -2432,7 +2432,7 @@
         <v>58</v>
       </c>
       <c r="B58" s="6" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="59" spans="1:2" x14ac:dyDescent="0.2">
@@ -2440,7 +2440,7 @@
         <v>59</v>
       </c>
       <c r="B59" s="6" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="60" spans="1:2" x14ac:dyDescent="0.2">
@@ -2448,7 +2448,7 @@
         <v>60</v>
       </c>
       <c r="B60" s="6" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="61" spans="1:2" x14ac:dyDescent="0.2">
@@ -2456,7 +2456,7 @@
         <v>61</v>
       </c>
       <c r="B61" s="6" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="62" spans="1:2" x14ac:dyDescent="0.2">
@@ -2464,7 +2464,7 @@
         <v>62</v>
       </c>
       <c r="B62" s="6" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="63" spans="1:2" x14ac:dyDescent="0.2">
@@ -2472,7 +2472,7 @@
         <v>63</v>
       </c>
       <c r="B63" s="6" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="64" spans="1:2" x14ac:dyDescent="0.2">
@@ -2486,7 +2486,7 @@
         <v>65</v>
       </c>
       <c r="B65" s="6" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="66" spans="1:2" x14ac:dyDescent="0.2">
@@ -2494,7 +2494,7 @@
         <v>66</v>
       </c>
       <c r="B66" s="6" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
   </sheetData>

</xml_diff>